<commit_message>
3d model test and updated parts list
</commit_message>
<xml_diff>
--- a/design_project_docs/parts_order.xlsx
+++ b/design_project_docs/parts_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dario\Documents\repos\Talit_Projekt_2024\design_project_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1149D852-81A1-429D-BBF0-EEAE48CA0C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD5EAA8-C1CB-4CD2-9B97-6360A68F5CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{CE665632-C620-4A27-B2F7-6BCB48880D40}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -507,7 +507,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>